<commit_message>
Updating data aggregation for new model fit approach
</commit_message>
<xml_diff>
--- a/model fit parameters.xlsx
+++ b/model fit parameters.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/UMN Google Drive/Research/Publications/Chapter 4/Version 2/GitHub/cndc_bayesian_eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21D189FC-C358-8046-B2E8-E80B1D4AC041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476D083-F5DF-6E41-AC46-8253052A7F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16780" yWindow="500" windowWidth="21820" windowHeight="16520" xr2:uid="{DA029428-0118-2E41-88AD-761AB8781422}"/>
+    <workbookView xWindow="6980" yWindow="6540" windowWidth="21820" windowHeight="10480" xr2:uid="{DA029428-0118-2E41-88AD-761AB8781422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -107,7 +107,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>